<commit_message>
Add oil pressure in bar and replace Kpa by Bar for fuel pressure
</commit_message>
<xml_diff>
--- a/STM2_ECU/SW/micro_to_mega_pinout.xlsx
+++ b/STM2_ECU/SW/micro_to_mega_pinout.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="231">
   <si>
     <t>MicroController pin</t>
   </si>
   <si>
-    <t>Feature in CfgEng</t>
-  </si>
-  <si>
-    <t>Feature in TestBench</t>
-  </si>
-  <si>
     <t>Mega pin</t>
   </si>
   <si>
@@ -521,6 +515,198 @@
   </si>
   <si>
     <t>AVCC</t>
+  </si>
+  <si>
+    <t>ECU_STM pin</t>
+  </si>
+  <si>
+    <t>Feature in ECU_STM</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>IACA2</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Aux1_DRV</t>
+  </si>
+  <si>
+    <t>FP_DRV</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>BOOST</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>INJ5</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>INJ3</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>INJ1</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>I NJ2</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>INJ4</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>IGN4</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>IGN2</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>IGN5</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>IGN1</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>IGN3</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>IACB2</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>IACB1</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>INJ6</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>IGN6</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>TACHO</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>DIG_IO2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>DIG_IO1</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>O2_1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>O2_2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>TPS</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>MAP_E</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>AI2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>AI1</t>
+  </si>
+  <si>
+    <t>CLT</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>MAT</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>TI1</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>TI2</t>
+  </si>
+  <si>
+    <t>K3</t>
   </si>
 </sst>
 </file>
@@ -897,34 +1083,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103:F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -932,10 +1119,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -943,10 +1130,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -954,10 +1141,10 @@
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -965,41 +1152,59 @@
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" t="s">
+        <v>169</v>
+      </c>
       <c r="D12" s="1">
         <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
       <c r="D13" s="1">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
       <c r="D14" s="1">
         <v>7</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -1007,7 +1212,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1016,352 +1221,442 @@
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" t="s">
+        <v>176</v>
+      </c>
       <c r="D19" s="1">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
       <c r="D20" s="1">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" t="s">
+        <v>180</v>
+      </c>
       <c r="D22" s="1">
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>182</v>
+      </c>
       <c r="D23" s="1">
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" t="s">
+        <v>184</v>
+      </c>
       <c r="D24" s="1">
         <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" t="s">
+        <v>186</v>
+      </c>
       <c r="D25" s="1">
         <v>18</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
       <c r="D26" s="1">
         <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>22</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" t="s">
+        <v>190</v>
+      </c>
       <c r="D30" s="1">
         <v>23</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" t="s">
+        <v>192</v>
+      </c>
       <c r="D31" s="1">
         <v>24</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" t="s">
+        <v>194</v>
+      </c>
       <c r="D32" s="1">
         <v>25</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" t="s">
+        <v>196</v>
+      </c>
       <c r="D33" s="1">
         <v>26</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <v>27</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>28</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>29</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D38" s="1">
         <v>31</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D39" s="1">
         <v>32</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
         <v>33</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D41" s="1">
         <v>34</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42" t="s">
+        <v>198</v>
+      </c>
       <c r="D42" s="1">
         <v>35</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>199</v>
+      </c>
+      <c r="C43" t="s">
+        <v>200</v>
+      </c>
       <c r="D43" s="1">
         <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>37</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D45" s="1">
         <v>38</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>202</v>
+      </c>
+      <c r="C46" t="s">
+        <v>203</v>
+      </c>
       <c r="D46" s="1">
         <v>39</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>204</v>
+      </c>
+      <c r="C47" t="s">
+        <v>205</v>
+      </c>
       <c r="D47" s="1">
         <v>40</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D48" s="1">
         <v>41</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.25">
@@ -1369,10 +1664,10 @@
         <v>42</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1380,10 +1675,10 @@
         <v>43</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1391,10 +1686,10 @@
         <v>44</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1402,10 +1697,10 @@
         <v>45</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1413,10 +1708,10 @@
         <v>46</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.25">
@@ -1424,7 +1719,7 @@
         <v>47</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -1433,7 +1728,7 @@
         <v>48</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -1442,7 +1737,7 @@
         <v>49</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -1451,10 +1746,10 @@
         <v>50</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.25">
@@ -1462,10 +1757,10 @@
         <v>51</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.25">
@@ -1473,10 +1768,10 @@
         <v>52</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
@@ -1484,10 +1779,10 @@
         <v>53</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.25">
@@ -1495,10 +1790,10 @@
         <v>54</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.25">
@@ -1506,10 +1801,10 @@
         <v>55</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.25">
@@ -1517,10 +1812,10 @@
         <v>56</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.25">
@@ -1528,10 +1823,10 @@
         <v>57</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
@@ -1539,10 +1834,10 @@
         <v>58</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
@@ -1550,10 +1845,10 @@
         <v>59</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
@@ -1561,10 +1856,10 @@
         <v>60</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
@@ -1572,10 +1867,10 @@
         <v>61</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
@@ -1583,10 +1878,10 @@
         <v>62</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1594,10 +1889,10 @@
         <v>63</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1605,10 +1900,10 @@
         <v>64</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
@@ -1616,7 +1911,7 @@
         <v>65</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F72" s="2"/>
     </row>
@@ -1625,7 +1920,7 @@
         <v>66</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F73" s="2"/>
     </row>
@@ -1634,7 +1929,7 @@
         <v>67</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F74" s="2"/>
     </row>
@@ -1643,7 +1938,7 @@
         <v>68</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F75" s="2"/>
     </row>
@@ -1652,7 +1947,7 @@
         <v>69</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F76" s="2"/>
     </row>
@@ -1661,10 +1956,10 @@
         <v>70</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.25">
@@ -1672,10 +1967,10 @@
         <v>71</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.25">
@@ -1683,10 +1978,10 @@
         <v>72</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.25">
@@ -1694,305 +1989,383 @@
         <v>73</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D81" s="1">
         <v>74</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D82" s="1">
         <v>75</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>206</v>
+      </c>
+      <c r="C83" t="s">
+        <v>207</v>
+      </c>
       <c r="D83" s="1">
         <v>76</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" t="s">
+        <v>209</v>
+      </c>
       <c r="D84" s="1">
         <v>77</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>210</v>
+      </c>
+      <c r="C85" t="s">
+        <v>211</v>
+      </c>
       <c r="D85" s="1">
         <v>78</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D86" s="1">
         <v>79</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D87" s="1">
         <v>80</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D88" s="1">
         <v>81</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="89" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D89" s="1">
         <v>82</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="90" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>212</v>
+      </c>
+      <c r="C90" t="s">
+        <v>213</v>
+      </c>
       <c r="D90" s="1">
         <v>83</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="91" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>214</v>
+      </c>
+      <c r="C91" t="s">
+        <v>215</v>
+      </c>
       <c r="D91" s="1">
         <v>84</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="92" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>216</v>
+      </c>
+      <c r="C92" t="s">
+        <v>217</v>
+      </c>
       <c r="D92" s="1">
         <v>85</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="93" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>218</v>
+      </c>
+      <c r="C93" t="s">
+        <v>219</v>
+      </c>
       <c r="D93" s="1">
         <v>86</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="94" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>220</v>
+      </c>
+      <c r="C94" t="s">
+        <v>221</v>
+      </c>
       <c r="D94" s="1">
         <v>87</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="95" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>222</v>
+      </c>
+      <c r="C95" t="s">
+        <v>201</v>
+      </c>
       <c r="D95" s="1">
         <v>88</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>223</v>
+      </c>
+      <c r="C96" t="s">
+        <v>224</v>
+      </c>
       <c r="D96" s="1">
         <v>89</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>225</v>
+      </c>
+      <c r="C97" t="s">
+        <v>226</v>
+      </c>
       <c r="D97" s="1">
         <v>90</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D98" s="1">
         <v>91</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D99" s="1">
         <v>92</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="100" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D100" s="1">
         <v>93</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D101" s="1">
         <v>94</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D102" s="1">
         <v>95</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" t="s">
+        <v>230</v>
+      </c>
       <c r="D103" s="1">
         <v>96</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="104" spans="4:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>227</v>
+      </c>
+      <c r="C104" t="s">
+        <v>228</v>
+      </c>
       <c r="D104" s="1">
         <v>97</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D105" s="1">
         <v>98</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D106" s="1">
         <v>99</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D107" s="1">
         <v>100</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>